<commit_message>
feat: add first ten cards parse
</commit_message>
<xml_diff>
--- a/Assets.xlsx
+++ b/Assets.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -445,7 +445,7 @@
         <v>SNW-Image0-01</v>
       </c>
       <c r="F2" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/2ac6a84713952960a18eb54cd3ed6b994342fabe/assets/SNW-0-01/0.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-0-01/0.jpg</v>
       </c>
       <c r="G2" t="str">
         <v>700</v>
@@ -471,7 +471,7 @@
         <v>SNW-Image0-02</v>
       </c>
       <c r="F3" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/2ac6a84713952960a18eb54cd3ed6b994342fabe/assets/SNW-0-01/1.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-0-01/1.jpg</v>
       </c>
       <c r="G3" t="str">
         <v>700</v>
@@ -497,7 +497,7 @@
         <v>SNW-Image0-03</v>
       </c>
       <c r="F4" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/2ac6a84713952960a18eb54cd3ed6b994342fabe/assets/SNW-0-01/2.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-0-01/2.jpg</v>
       </c>
       <c r="G4" t="str">
         <v>700</v>
@@ -523,7 +523,7 @@
         <v>SNW-Image0-04</v>
       </c>
       <c r="F5" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/2ac6a84713952960a18eb54cd3ed6b994342fabe/assets/SNW-0-01/3.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-0-01/3.jpg</v>
       </c>
       <c r="G5" t="str">
         <v>700</v>
@@ -549,7 +549,7 @@
         <v>SNW-Image0-05</v>
       </c>
       <c r="F6" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/2ac6a84713952960a18eb54cd3ed6b994342fabe/assets/SNW-0-01/4.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-0-01/4.jpg</v>
       </c>
       <c r="G6" t="str">
         <v>700</v>
@@ -575,7 +575,7 @@
         <v>SNW-Image1-01</v>
       </c>
       <c r="F7" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/2ac6a84713952960a18eb54cd3ed6b994342fabe/assets/SNW-1-01/0.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-1-01/0.jpg</v>
       </c>
       <c r="G7" t="str">
         <v>700</v>
@@ -601,7 +601,7 @@
         <v>SNW-Image1-02</v>
       </c>
       <c r="F8" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/2ac6a84713952960a18eb54cd3ed6b994342fabe/assets/SNW-1-01/1.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-1-01/1.jpg</v>
       </c>
       <c r="G8" t="str">
         <v>700</v>
@@ -627,7 +627,7 @@
         <v>SNW-Image1-03</v>
       </c>
       <c r="F9" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/2ac6a84713952960a18eb54cd3ed6b994342fabe/assets/SNW-1-01/2.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-1-01/2.jpg</v>
       </c>
       <c r="G9" t="str">
         <v>700</v>
@@ -653,7 +653,7 @@
         <v>SNW-Image1-04</v>
       </c>
       <c r="F10" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/2ac6a84713952960a18eb54cd3ed6b994342fabe/assets/SNW-1-01/3.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-1-01/3.jpg</v>
       </c>
       <c r="G10" t="str">
         <v>700</v>
@@ -679,18 +679,1058 @@
         <v>SNW-Image1-05</v>
       </c>
       <c r="F11" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/2ac6a84713952960a18eb54cd3ed6b994342fabe/assets/SNW-1-01/4.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-1-01/4.jpg</v>
       </c>
       <c r="G11" t="str">
         <v>700</v>
       </c>
       <c r="H11" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>image</v>
+      </c>
+      <c r="B12" t="str">
+        <v>snowboard102</v>
+      </c>
+      <c r="C12" t="str">
+        <v>SNW-2537-01</v>
+      </c>
+      <c r="D12" t="str">
+        <v>SNW-2-01</v>
+      </c>
+      <c r="E12" t="str">
+        <v>SNW-Image2-01</v>
+      </c>
+      <c r="F12" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-2-01/0.jpg</v>
+      </c>
+      <c r="G12" t="str">
+        <v>700</v>
+      </c>
+      <c r="H12" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>image</v>
+      </c>
+      <c r="B13" t="str">
+        <v>snowboard102</v>
+      </c>
+      <c r="C13" t="str">
+        <v>SNW-2537-01</v>
+      </c>
+      <c r="D13" t="str">
+        <v>SNW-2-01</v>
+      </c>
+      <c r="E13" t="str">
+        <v>SNW-Image2-02</v>
+      </c>
+      <c r="F13" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-2-01/1.jpg</v>
+      </c>
+      <c r="G13" t="str">
+        <v>700</v>
+      </c>
+      <c r="H13" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>image</v>
+      </c>
+      <c r="B14" t="str">
+        <v>snowboard102</v>
+      </c>
+      <c r="C14" t="str">
+        <v>SNW-2537-01</v>
+      </c>
+      <c r="D14" t="str">
+        <v>SNW-2-01</v>
+      </c>
+      <c r="E14" t="str">
+        <v>SNW-Image2-03</v>
+      </c>
+      <c r="F14" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-2-01/2.jpg</v>
+      </c>
+      <c r="G14" t="str">
+        <v>700</v>
+      </c>
+      <c r="H14" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>image</v>
+      </c>
+      <c r="B15" t="str">
+        <v>snowboard102</v>
+      </c>
+      <c r="C15" t="str">
+        <v>SNW-2537-01</v>
+      </c>
+      <c r="D15" t="str">
+        <v>SNW-2-01</v>
+      </c>
+      <c r="E15" t="str">
+        <v>SNW-Image2-04</v>
+      </c>
+      <c r="F15" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-2-01/3.jpg</v>
+      </c>
+      <c r="G15" t="str">
+        <v>700</v>
+      </c>
+      <c r="H15" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>image</v>
+      </c>
+      <c r="B16" t="str">
+        <v>snowboard102</v>
+      </c>
+      <c r="C16" t="str">
+        <v>SNW-2537-01</v>
+      </c>
+      <c r="D16" t="str">
+        <v>SNW-2-01</v>
+      </c>
+      <c r="E16" t="str">
+        <v>SNW-Image2-05</v>
+      </c>
+      <c r="F16" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-2-01/4.jpg</v>
+      </c>
+      <c r="G16" t="str">
+        <v>700</v>
+      </c>
+      <c r="H16" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>image</v>
+      </c>
+      <c r="B17" t="str">
+        <v>snowboard103</v>
+      </c>
+      <c r="C17" t="str">
+        <v>SNW-2155-01</v>
+      </c>
+      <c r="D17" t="str">
+        <v>SNW-3-01</v>
+      </c>
+      <c r="E17" t="str">
+        <v>SNW-Image3-01</v>
+      </c>
+      <c r="F17" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-3-01/0.jpg</v>
+      </c>
+      <c r="G17" t="str">
+        <v>700</v>
+      </c>
+      <c r="H17" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>image</v>
+      </c>
+      <c r="B18" t="str">
+        <v>snowboard103</v>
+      </c>
+      <c r="C18" t="str">
+        <v>SNW-2155-01</v>
+      </c>
+      <c r="D18" t="str">
+        <v>SNW-3-01</v>
+      </c>
+      <c r="E18" t="str">
+        <v>SNW-Image3-02</v>
+      </c>
+      <c r="F18" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-3-01/1.jpg</v>
+      </c>
+      <c r="G18" t="str">
+        <v>700</v>
+      </c>
+      <c r="H18" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>image</v>
+      </c>
+      <c r="B19" t="str">
+        <v>snowboard103</v>
+      </c>
+      <c r="C19" t="str">
+        <v>SNW-2155-01</v>
+      </c>
+      <c r="D19" t="str">
+        <v>SNW-3-01</v>
+      </c>
+      <c r="E19" t="str">
+        <v>SNW-Image3-03</v>
+      </c>
+      <c r="F19" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-3-01/2.jpg</v>
+      </c>
+      <c r="G19" t="str">
+        <v>700</v>
+      </c>
+      <c r="H19" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>image</v>
+      </c>
+      <c r="B20" t="str">
+        <v>snowboard103</v>
+      </c>
+      <c r="C20" t="str">
+        <v>SNW-2155-01</v>
+      </c>
+      <c r="D20" t="str">
+        <v>SNW-3-01</v>
+      </c>
+      <c r="E20" t="str">
+        <v>SNW-Image3-04</v>
+      </c>
+      <c r="F20" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-3-01/3.jpg</v>
+      </c>
+      <c r="G20" t="str">
+        <v>700</v>
+      </c>
+      <c r="H20" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>image</v>
+      </c>
+      <c r="B21" t="str">
+        <v>snowboard103</v>
+      </c>
+      <c r="C21" t="str">
+        <v>SNW-2155-01</v>
+      </c>
+      <c r="D21" t="str">
+        <v>SNW-3-01</v>
+      </c>
+      <c r="E21" t="str">
+        <v>SNW-Image3-05</v>
+      </c>
+      <c r="F21" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-3-01/4.jpg</v>
+      </c>
+      <c r="G21" t="str">
+        <v>700</v>
+      </c>
+      <c r="H21" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>image</v>
+      </c>
+      <c r="B22" t="str">
+        <v>snowboard104</v>
+      </c>
+      <c r="C22" t="str">
+        <v>SNW-2876-01</v>
+      </c>
+      <c r="D22" t="str">
+        <v>SNW-4-01</v>
+      </c>
+      <c r="E22" t="str">
+        <v>SNW-Image4-01</v>
+      </c>
+      <c r="F22" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-4-01/0.jpg</v>
+      </c>
+      <c r="G22" t="str">
+        <v>700</v>
+      </c>
+      <c r="H22" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>image</v>
+      </c>
+      <c r="B23" t="str">
+        <v>snowboard104</v>
+      </c>
+      <c r="C23" t="str">
+        <v>SNW-2876-01</v>
+      </c>
+      <c r="D23" t="str">
+        <v>SNW-4-01</v>
+      </c>
+      <c r="E23" t="str">
+        <v>SNW-Image4-02</v>
+      </c>
+      <c r="F23" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-4-01/1.jpg</v>
+      </c>
+      <c r="G23" t="str">
+        <v>700</v>
+      </c>
+      <c r="H23" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>image</v>
+      </c>
+      <c r="B24" t="str">
+        <v>snowboard104</v>
+      </c>
+      <c r="C24" t="str">
+        <v>SNW-2876-01</v>
+      </c>
+      <c r="D24" t="str">
+        <v>SNW-4-01</v>
+      </c>
+      <c r="E24" t="str">
+        <v>SNW-Image4-03</v>
+      </c>
+      <c r="F24" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-4-01/2.jpg</v>
+      </c>
+      <c r="G24" t="str">
+        <v>700</v>
+      </c>
+      <c r="H24" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>image</v>
+      </c>
+      <c r="B25" t="str">
+        <v>snowboard104</v>
+      </c>
+      <c r="C25" t="str">
+        <v>SNW-2876-01</v>
+      </c>
+      <c r="D25" t="str">
+        <v>SNW-4-01</v>
+      </c>
+      <c r="E25" t="str">
+        <v>SNW-Image4-04</v>
+      </c>
+      <c r="F25" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-4-01/3.jpg</v>
+      </c>
+      <c r="G25" t="str">
+        <v>700</v>
+      </c>
+      <c r="H25" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>image</v>
+      </c>
+      <c r="B26" t="str">
+        <v>snowboard104</v>
+      </c>
+      <c r="C26" t="str">
+        <v>SNW-2876-01</v>
+      </c>
+      <c r="D26" t="str">
+        <v>SNW-4-01</v>
+      </c>
+      <c r="E26" t="str">
+        <v>SNW-Image4-05</v>
+      </c>
+      <c r="F26" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-4-01/4.jpg</v>
+      </c>
+      <c r="G26" t="str">
+        <v>700</v>
+      </c>
+      <c r="H26" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>image</v>
+      </c>
+      <c r="B27" t="str">
+        <v>snowboard105</v>
+      </c>
+      <c r="C27" t="str">
+        <v>SNW-3398-01</v>
+      </c>
+      <c r="D27" t="str">
+        <v>SNW-5-01</v>
+      </c>
+      <c r="E27" t="str">
+        <v>SNW-Image5-01</v>
+      </c>
+      <c r="F27" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-5-01/0.jpg</v>
+      </c>
+      <c r="G27" t="str">
+        <v>700</v>
+      </c>
+      <c r="H27" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>image</v>
+      </c>
+      <c r="B28" t="str">
+        <v>snowboard105</v>
+      </c>
+      <c r="C28" t="str">
+        <v>SNW-3398-01</v>
+      </c>
+      <c r="D28" t="str">
+        <v>SNW-5-01</v>
+      </c>
+      <c r="E28" t="str">
+        <v>SNW-Image5-02</v>
+      </c>
+      <c r="F28" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-5-01/1.jpg</v>
+      </c>
+      <c r="G28" t="str">
+        <v>700</v>
+      </c>
+      <c r="H28" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>image</v>
+      </c>
+      <c r="B29" t="str">
+        <v>snowboard105</v>
+      </c>
+      <c r="C29" t="str">
+        <v>SNW-3398-01</v>
+      </c>
+      <c r="D29" t="str">
+        <v>SNW-5-01</v>
+      </c>
+      <c r="E29" t="str">
+        <v>SNW-Image5-03</v>
+      </c>
+      <c r="F29" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-5-01/2.jpg</v>
+      </c>
+      <c r="G29" t="str">
+        <v>700</v>
+      </c>
+      <c r="H29" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>image</v>
+      </c>
+      <c r="B30" t="str">
+        <v>snowboard105</v>
+      </c>
+      <c r="C30" t="str">
+        <v>SNW-3398-01</v>
+      </c>
+      <c r="D30" t="str">
+        <v>SNW-5-01</v>
+      </c>
+      <c r="E30" t="str">
+        <v>SNW-Image5-04</v>
+      </c>
+      <c r="F30" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-5-01/3.jpg</v>
+      </c>
+      <c r="G30" t="str">
+        <v>700</v>
+      </c>
+      <c r="H30" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>image</v>
+      </c>
+      <c r="B31" t="str">
+        <v>snowboard105</v>
+      </c>
+      <c r="C31" t="str">
+        <v>SNW-3398-01</v>
+      </c>
+      <c r="D31" t="str">
+        <v>SNW-5-01</v>
+      </c>
+      <c r="E31" t="str">
+        <v>SNW-Image5-05</v>
+      </c>
+      <c r="F31" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-5-01/4.jpg</v>
+      </c>
+      <c r="G31" t="str">
+        <v>700</v>
+      </c>
+      <c r="H31" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>image</v>
+      </c>
+      <c r="B32" t="str">
+        <v>snowboard106</v>
+      </c>
+      <c r="C32" t="str">
+        <v>SNW-2245-01</v>
+      </c>
+      <c r="D32" t="str">
+        <v>SNW-6-01</v>
+      </c>
+      <c r="E32" t="str">
+        <v>SNW-Image6-01</v>
+      </c>
+      <c r="F32" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-6-01/0.jpg</v>
+      </c>
+      <c r="G32" t="str">
+        <v>700</v>
+      </c>
+      <c r="H32" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>image</v>
+      </c>
+      <c r="B33" t="str">
+        <v>snowboard106</v>
+      </c>
+      <c r="C33" t="str">
+        <v>SNW-2245-01</v>
+      </c>
+      <c r="D33" t="str">
+        <v>SNW-6-01</v>
+      </c>
+      <c r="E33" t="str">
+        <v>SNW-Image6-02</v>
+      </c>
+      <c r="F33" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-6-01/1.jpg</v>
+      </c>
+      <c r="G33" t="str">
+        <v>700</v>
+      </c>
+      <c r="H33" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>image</v>
+      </c>
+      <c r="B34" t="str">
+        <v>snowboard106</v>
+      </c>
+      <c r="C34" t="str">
+        <v>SNW-2245-01</v>
+      </c>
+      <c r="D34" t="str">
+        <v>SNW-6-01</v>
+      </c>
+      <c r="E34" t="str">
+        <v>SNW-Image6-03</v>
+      </c>
+      <c r="F34" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-6-01/2.jpg</v>
+      </c>
+      <c r="G34" t="str">
+        <v>700</v>
+      </c>
+      <c r="H34" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>image</v>
+      </c>
+      <c r="B35" t="str">
+        <v>snowboard106</v>
+      </c>
+      <c r="C35" t="str">
+        <v>SNW-2245-01</v>
+      </c>
+      <c r="D35" t="str">
+        <v>SNW-6-01</v>
+      </c>
+      <c r="E35" t="str">
+        <v>SNW-Image6-04</v>
+      </c>
+      <c r="F35" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-6-01/3.jpg</v>
+      </c>
+      <c r="G35" t="str">
+        <v>700</v>
+      </c>
+      <c r="H35" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>image</v>
+      </c>
+      <c r="B36" t="str">
+        <v>snowboard106</v>
+      </c>
+      <c r="C36" t="str">
+        <v>SNW-2245-01</v>
+      </c>
+      <c r="D36" t="str">
+        <v>SNW-6-01</v>
+      </c>
+      <c r="E36" t="str">
+        <v>SNW-Image6-05</v>
+      </c>
+      <c r="F36" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-6-01/4.jpg</v>
+      </c>
+      <c r="G36" t="str">
+        <v>700</v>
+      </c>
+      <c r="H36" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>image</v>
+      </c>
+      <c r="B37" t="str">
+        <v>snowboard107</v>
+      </c>
+      <c r="C37" t="str">
+        <v>SNW-2905-01</v>
+      </c>
+      <c r="D37" t="str">
+        <v>SNW-7-01</v>
+      </c>
+      <c r="E37" t="str">
+        <v>SNW-Image7-01</v>
+      </c>
+      <c r="F37" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-7-01/0.jpg</v>
+      </c>
+      <c r="G37" t="str">
+        <v>700</v>
+      </c>
+      <c r="H37" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>image</v>
+      </c>
+      <c r="B38" t="str">
+        <v>snowboard107</v>
+      </c>
+      <c r="C38" t="str">
+        <v>SNW-2905-01</v>
+      </c>
+      <c r="D38" t="str">
+        <v>SNW-7-01</v>
+      </c>
+      <c r="E38" t="str">
+        <v>SNW-Image7-02</v>
+      </c>
+      <c r="F38" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-7-01/1.jpg</v>
+      </c>
+      <c r="G38" t="str">
+        <v>700</v>
+      </c>
+      <c r="H38" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>image</v>
+      </c>
+      <c r="B39" t="str">
+        <v>snowboard107</v>
+      </c>
+      <c r="C39" t="str">
+        <v>SNW-2905-01</v>
+      </c>
+      <c r="D39" t="str">
+        <v>SNW-7-01</v>
+      </c>
+      <c r="E39" t="str">
+        <v>SNW-Image7-03</v>
+      </c>
+      <c r="F39" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-7-01/2.jpg</v>
+      </c>
+      <c r="G39" t="str">
+        <v>700</v>
+      </c>
+      <c r="H39" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>image</v>
+      </c>
+      <c r="B40" t="str">
+        <v>snowboard107</v>
+      </c>
+      <c r="C40" t="str">
+        <v>SNW-2905-01</v>
+      </c>
+      <c r="D40" t="str">
+        <v>SNW-7-01</v>
+      </c>
+      <c r="E40" t="str">
+        <v>SNW-Image7-04</v>
+      </c>
+      <c r="F40" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-7-01/3.jpg</v>
+      </c>
+      <c r="G40" t="str">
+        <v>700</v>
+      </c>
+      <c r="H40" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>image</v>
+      </c>
+      <c r="B41" t="str">
+        <v>snowboard107</v>
+      </c>
+      <c r="C41" t="str">
+        <v>SNW-2905-01</v>
+      </c>
+      <c r="D41" t="str">
+        <v>SNW-7-01</v>
+      </c>
+      <c r="E41" t="str">
+        <v>SNW-Image7-05</v>
+      </c>
+      <c r="F41" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-7-01/4.jpg</v>
+      </c>
+      <c r="G41" t="str">
+        <v>700</v>
+      </c>
+      <c r="H41" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>image</v>
+      </c>
+      <c r="B42" t="str">
+        <v>snowboard108</v>
+      </c>
+      <c r="C42" t="str">
+        <v>SNW-3162-01</v>
+      </c>
+      <c r="D42" t="str">
+        <v>SNW-8-01</v>
+      </c>
+      <c r="E42" t="str">
+        <v>SNW-Image8-01</v>
+      </c>
+      <c r="F42" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-8-01/0.jpg</v>
+      </c>
+      <c r="G42" t="str">
+        <v>700</v>
+      </c>
+      <c r="H42" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>image</v>
+      </c>
+      <c r="B43" t="str">
+        <v>snowboard108</v>
+      </c>
+      <c r="C43" t="str">
+        <v>SNW-3162-01</v>
+      </c>
+      <c r="D43" t="str">
+        <v>SNW-8-01</v>
+      </c>
+      <c r="E43" t="str">
+        <v>SNW-Image8-02</v>
+      </c>
+      <c r="F43" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-8-01/1.jpg</v>
+      </c>
+      <c r="G43" t="str">
+        <v>700</v>
+      </c>
+      <c r="H43" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>image</v>
+      </c>
+      <c r="B44" t="str">
+        <v>snowboard108</v>
+      </c>
+      <c r="C44" t="str">
+        <v>SNW-3162-01</v>
+      </c>
+      <c r="D44" t="str">
+        <v>SNW-8-01</v>
+      </c>
+      <c r="E44" t="str">
+        <v>SNW-Image8-03</v>
+      </c>
+      <c r="F44" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-8-01/2.jpg</v>
+      </c>
+      <c r="G44" t="str">
+        <v>700</v>
+      </c>
+      <c r="H44" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>image</v>
+      </c>
+      <c r="B45" t="str">
+        <v>snowboard108</v>
+      </c>
+      <c r="C45" t="str">
+        <v>SNW-3162-01</v>
+      </c>
+      <c r="D45" t="str">
+        <v>SNW-8-01</v>
+      </c>
+      <c r="E45" t="str">
+        <v>SNW-Image8-04</v>
+      </c>
+      <c r="F45" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-8-01/3.jpg</v>
+      </c>
+      <c r="G45" t="str">
+        <v>700</v>
+      </c>
+      <c r="H45" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>image</v>
+      </c>
+      <c r="B46" t="str">
+        <v>snowboard108</v>
+      </c>
+      <c r="C46" t="str">
+        <v>SNW-3162-01</v>
+      </c>
+      <c r="D46" t="str">
+        <v>SNW-8-01</v>
+      </c>
+      <c r="E46" t="str">
+        <v>SNW-Image8-05</v>
+      </c>
+      <c r="F46" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-8-01/4.jpg</v>
+      </c>
+      <c r="G46" t="str">
+        <v>700</v>
+      </c>
+      <c r="H46" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>image</v>
+      </c>
+      <c r="B47" t="str">
+        <v>snowboard109</v>
+      </c>
+      <c r="C47" t="str">
+        <v>SNW-2858-01</v>
+      </c>
+      <c r="D47" t="str">
+        <v>SNW-9-01</v>
+      </c>
+      <c r="E47" t="str">
+        <v>SNW-Image9-01</v>
+      </c>
+      <c r="F47" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-9-01/0.jpg</v>
+      </c>
+      <c r="G47" t="str">
+        <v>700</v>
+      </c>
+      <c r="H47" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>image</v>
+      </c>
+      <c r="B48" t="str">
+        <v>snowboard109</v>
+      </c>
+      <c r="C48" t="str">
+        <v>SNW-2858-01</v>
+      </c>
+      <c r="D48" t="str">
+        <v>SNW-9-01</v>
+      </c>
+      <c r="E48" t="str">
+        <v>SNW-Image9-02</v>
+      </c>
+      <c r="F48" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-9-01/1.jpg</v>
+      </c>
+      <c r="G48" t="str">
+        <v>700</v>
+      </c>
+      <c r="H48" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>image</v>
+      </c>
+      <c r="B49" t="str">
+        <v>snowboard109</v>
+      </c>
+      <c r="C49" t="str">
+        <v>SNW-2858-01</v>
+      </c>
+      <c r="D49" t="str">
+        <v>SNW-9-01</v>
+      </c>
+      <c r="E49" t="str">
+        <v>SNW-Image9-03</v>
+      </c>
+      <c r="F49" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-9-01/2.jpg</v>
+      </c>
+      <c r="G49" t="str">
+        <v>700</v>
+      </c>
+      <c r="H49" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>image</v>
+      </c>
+      <c r="B50" t="str">
+        <v>snowboard109</v>
+      </c>
+      <c r="C50" t="str">
+        <v>SNW-2858-01</v>
+      </c>
+      <c r="D50" t="str">
+        <v>SNW-9-01</v>
+      </c>
+      <c r="E50" t="str">
+        <v>SNW-Image9-04</v>
+      </c>
+      <c r="F50" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-9-01/3.jpg</v>
+      </c>
+      <c r="G50" t="str">
+        <v>700</v>
+      </c>
+      <c r="H50" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>image</v>
+      </c>
+      <c r="B51" t="str">
+        <v>snowboard109</v>
+      </c>
+      <c r="C51" t="str">
+        <v>SNW-2858-01</v>
+      </c>
+      <c r="D51" t="str">
+        <v>SNW-9-01</v>
+      </c>
+      <c r="E51" t="str">
+        <v>SNW-Image9-05</v>
+      </c>
+      <c r="F51" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-9-01/4.jpg</v>
+      </c>
+      <c r="G51" t="str">
+        <v>700</v>
+      </c>
+      <c r="H51" t="str">
         <v>700</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H51"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: fix processing cases of borderline number of pictures per card
</commit_message>
<xml_diff>
--- a/Assets.xlsx
+++ b/Assets.xlsx
@@ -397,10 +397,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="8" max="8" width="5.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -719,19 +723,19 @@
         <v>image</v>
       </c>
       <c r="B13" t="str">
-        <v>snowboard102</v>
+        <v>snowboard103</v>
       </c>
       <c r="C13" t="str">
-        <v>SNW-2537-01</v>
+        <v>SNW-2155-01</v>
       </c>
       <c r="D13" t="str">
-        <v>SNW-2-01</v>
+        <v>SNW-3-01</v>
       </c>
       <c r="E13" t="str">
-        <v>SNW-Image2-02</v>
+        <v>SNW-Image3-01</v>
       </c>
       <c r="F13" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-2-01/1.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-3-01/0.jpg</v>
       </c>
       <c r="G13" t="str">
         <v>700</v>
@@ -745,19 +749,19 @@
         <v>image</v>
       </c>
       <c r="B14" t="str">
-        <v>snowboard102</v>
+        <v>snowboard103</v>
       </c>
       <c r="C14" t="str">
-        <v>SNW-2537-01</v>
+        <v>SNW-2155-01</v>
       </c>
       <c r="D14" t="str">
-        <v>SNW-2-01</v>
+        <v>SNW-3-01</v>
       </c>
       <c r="E14" t="str">
-        <v>SNW-Image2-03</v>
+        <v>SNW-Image3-02</v>
       </c>
       <c r="F14" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-2-01/2.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-3-01/1.jpg</v>
       </c>
       <c r="G14" t="str">
         <v>700</v>
@@ -771,19 +775,19 @@
         <v>image</v>
       </c>
       <c r="B15" t="str">
-        <v>snowboard102</v>
+        <v>snowboard103</v>
       </c>
       <c r="C15" t="str">
-        <v>SNW-2537-01</v>
+        <v>SNW-2155-01</v>
       </c>
       <c r="D15" t="str">
-        <v>SNW-2-01</v>
+        <v>SNW-3-01</v>
       </c>
       <c r="E15" t="str">
-        <v>SNW-Image2-04</v>
+        <v>SNW-Image3-03</v>
       </c>
       <c r="F15" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-2-01/3.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-3-01/2.jpg</v>
       </c>
       <c r="G15" t="str">
         <v>700</v>
@@ -797,19 +801,19 @@
         <v>image</v>
       </c>
       <c r="B16" t="str">
-        <v>snowboard102</v>
+        <v>snowboard103</v>
       </c>
       <c r="C16" t="str">
-        <v>SNW-2537-01</v>
+        <v>SNW-2155-01</v>
       </c>
       <c r="D16" t="str">
-        <v>SNW-2-01</v>
+        <v>SNW-3-01</v>
       </c>
       <c r="E16" t="str">
-        <v>SNW-Image2-05</v>
+        <v>SNW-Image3-04</v>
       </c>
       <c r="F16" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-2-01/4.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-3-01/3.jpg</v>
       </c>
       <c r="G16" t="str">
         <v>700</v>
@@ -832,10 +836,10 @@
         <v>SNW-3-01</v>
       </c>
       <c r="E17" t="str">
-        <v>SNW-Image3-01</v>
+        <v>SNW-Image3-05</v>
       </c>
       <c r="F17" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-3-01/0.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-3-01/4.jpg</v>
       </c>
       <c r="G17" t="str">
         <v>700</v>
@@ -849,19 +853,19 @@
         <v>image</v>
       </c>
       <c r="B18" t="str">
-        <v>snowboard103</v>
+        <v>snowboard104</v>
       </c>
       <c r="C18" t="str">
-        <v>SNW-2155-01</v>
+        <v>SNW-2876-01</v>
       </c>
       <c r="D18" t="str">
-        <v>SNW-3-01</v>
+        <v>SNW-4-01</v>
       </c>
       <c r="E18" t="str">
-        <v>SNW-Image3-02</v>
+        <v>SNW-Image4-01</v>
       </c>
       <c r="F18" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-3-01/1.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-4-01/0.jpg</v>
       </c>
       <c r="G18" t="str">
         <v>700</v>
@@ -875,19 +879,19 @@
         <v>image</v>
       </c>
       <c r="B19" t="str">
-        <v>snowboard103</v>
+        <v>snowboard104</v>
       </c>
       <c r="C19" t="str">
-        <v>SNW-2155-01</v>
+        <v>SNW-2876-01</v>
       </c>
       <c r="D19" t="str">
-        <v>SNW-3-01</v>
+        <v>SNW-4-01</v>
       </c>
       <c r="E19" t="str">
-        <v>SNW-Image3-03</v>
+        <v>SNW-Image4-02</v>
       </c>
       <c r="F19" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-3-01/2.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-4-01/1.jpg</v>
       </c>
       <c r="G19" t="str">
         <v>700</v>
@@ -901,19 +905,19 @@
         <v>image</v>
       </c>
       <c r="B20" t="str">
-        <v>snowboard103</v>
+        <v>snowboard104</v>
       </c>
       <c r="C20" t="str">
-        <v>SNW-2155-01</v>
+        <v>SNW-2876-01</v>
       </c>
       <c r="D20" t="str">
-        <v>SNW-3-01</v>
+        <v>SNW-4-01</v>
       </c>
       <c r="E20" t="str">
-        <v>SNW-Image3-04</v>
+        <v>SNW-Image4-03</v>
       </c>
       <c r="F20" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-3-01/3.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-4-01/2.jpg</v>
       </c>
       <c r="G20" t="str">
         <v>700</v>
@@ -927,19 +931,19 @@
         <v>image</v>
       </c>
       <c r="B21" t="str">
-        <v>snowboard103</v>
+        <v>snowboard104</v>
       </c>
       <c r="C21" t="str">
-        <v>SNW-2155-01</v>
+        <v>SNW-2876-01</v>
       </c>
       <c r="D21" t="str">
-        <v>SNW-3-01</v>
+        <v>SNW-4-01</v>
       </c>
       <c r="E21" t="str">
-        <v>SNW-Image3-05</v>
+        <v>SNW-Image4-04</v>
       </c>
       <c r="F21" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-3-01/4.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-4-01/3.jpg</v>
       </c>
       <c r="G21" t="str">
         <v>700</v>
@@ -962,10 +966,10 @@
         <v>SNW-4-01</v>
       </c>
       <c r="E22" t="str">
-        <v>SNW-Image4-01</v>
+        <v>SNW-Image4-05</v>
       </c>
       <c r="F22" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-4-01/0.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-4-01/4.jpg</v>
       </c>
       <c r="G22" t="str">
         <v>700</v>
@@ -979,19 +983,19 @@
         <v>image</v>
       </c>
       <c r="B23" t="str">
-        <v>snowboard104</v>
+        <v>snowboard105</v>
       </c>
       <c r="C23" t="str">
-        <v>SNW-2876-01</v>
+        <v>SNW-3398-01</v>
       </c>
       <c r="D23" t="str">
-        <v>SNW-4-01</v>
+        <v>SNW-5-01</v>
       </c>
       <c r="E23" t="str">
-        <v>SNW-Image4-02</v>
+        <v>SNW-Image5-01</v>
       </c>
       <c r="F23" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-4-01/1.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-5-01/0.jpg</v>
       </c>
       <c r="G23" t="str">
         <v>700</v>
@@ -1005,19 +1009,19 @@
         <v>image</v>
       </c>
       <c r="B24" t="str">
-        <v>snowboard104</v>
+        <v>snowboard105</v>
       </c>
       <c r="C24" t="str">
-        <v>SNW-2876-01</v>
+        <v>SNW-3398-01</v>
       </c>
       <c r="D24" t="str">
-        <v>SNW-4-01</v>
+        <v>SNW-5-01</v>
       </c>
       <c r="E24" t="str">
-        <v>SNW-Image4-03</v>
+        <v>SNW-Image5-02</v>
       </c>
       <c r="F24" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-4-01/2.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-5-01/1.jpg</v>
       </c>
       <c r="G24" t="str">
         <v>700</v>
@@ -1031,19 +1035,19 @@
         <v>image</v>
       </c>
       <c r="B25" t="str">
-        <v>snowboard104</v>
+        <v>snowboard105</v>
       </c>
       <c r="C25" t="str">
-        <v>SNW-2876-01</v>
+        <v>SNW-3398-01</v>
       </c>
       <c r="D25" t="str">
-        <v>SNW-4-01</v>
+        <v>SNW-5-01</v>
       </c>
       <c r="E25" t="str">
-        <v>SNW-Image4-04</v>
+        <v>SNW-Image5-03</v>
       </c>
       <c r="F25" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-4-01/3.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-5-01/2.jpg</v>
       </c>
       <c r="G25" t="str">
         <v>700</v>
@@ -1057,19 +1061,19 @@
         <v>image</v>
       </c>
       <c r="B26" t="str">
-        <v>snowboard104</v>
+        <v>snowboard106</v>
       </c>
       <c r="C26" t="str">
-        <v>SNW-2876-01</v>
+        <v>SNW-2245-01</v>
       </c>
       <c r="D26" t="str">
-        <v>SNW-4-01</v>
+        <v>SNW-6-01</v>
       </c>
       <c r="E26" t="str">
-        <v>SNW-Image4-05</v>
+        <v>SNW-Image6-01</v>
       </c>
       <c r="F26" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-4-01/4.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-6-01/0.jpg</v>
       </c>
       <c r="G26" t="str">
         <v>700</v>
@@ -1083,19 +1087,19 @@
         <v>image</v>
       </c>
       <c r="B27" t="str">
-        <v>snowboard105</v>
+        <v>snowboard106</v>
       </c>
       <c r="C27" t="str">
-        <v>SNW-3398-01</v>
+        <v>SNW-2245-01</v>
       </c>
       <c r="D27" t="str">
-        <v>SNW-5-01</v>
+        <v>SNW-6-01</v>
       </c>
       <c r="E27" t="str">
-        <v>SNW-Image5-01</v>
+        <v>SNW-Image6-02</v>
       </c>
       <c r="F27" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-5-01/0.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-6-01/1.jpg</v>
       </c>
       <c r="G27" t="str">
         <v>700</v>
@@ -1109,19 +1113,19 @@
         <v>image</v>
       </c>
       <c r="B28" t="str">
-        <v>snowboard105</v>
+        <v>snowboard106</v>
       </c>
       <c r="C28" t="str">
-        <v>SNW-3398-01</v>
+        <v>SNW-2245-01</v>
       </c>
       <c r="D28" t="str">
-        <v>SNW-5-01</v>
+        <v>SNW-6-01</v>
       </c>
       <c r="E28" t="str">
-        <v>SNW-Image5-02</v>
+        <v>SNW-Image6-03</v>
       </c>
       <c r="F28" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-5-01/1.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-6-01/2.jpg</v>
       </c>
       <c r="G28" t="str">
         <v>700</v>
@@ -1135,19 +1139,19 @@
         <v>image</v>
       </c>
       <c r="B29" t="str">
-        <v>snowboard105</v>
+        <v>snowboard106</v>
       </c>
       <c r="C29" t="str">
-        <v>SNW-3398-01</v>
+        <v>SNW-2245-01</v>
       </c>
       <c r="D29" t="str">
-        <v>SNW-5-01</v>
+        <v>SNW-6-01</v>
       </c>
       <c r="E29" t="str">
-        <v>SNW-Image5-03</v>
+        <v>SNW-Image6-04</v>
       </c>
       <c r="F29" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-5-01/2.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-6-01/3.jpg</v>
       </c>
       <c r="G29" t="str">
         <v>700</v>
@@ -1161,19 +1165,19 @@
         <v>image</v>
       </c>
       <c r="B30" t="str">
-        <v>snowboard105</v>
+        <v>snowboard106</v>
       </c>
       <c r="C30" t="str">
-        <v>SNW-3398-01</v>
+        <v>SNW-2245-01</v>
       </c>
       <c r="D30" t="str">
-        <v>SNW-5-01</v>
+        <v>SNW-6-01</v>
       </c>
       <c r="E30" t="str">
-        <v>SNW-Image5-04</v>
+        <v>SNW-Image6-05</v>
       </c>
       <c r="F30" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-5-01/3.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-6-01/4.jpg</v>
       </c>
       <c r="G30" t="str">
         <v>700</v>
@@ -1187,19 +1191,19 @@
         <v>image</v>
       </c>
       <c r="B31" t="str">
-        <v>snowboard105</v>
+        <v>snowboard107</v>
       </c>
       <c r="C31" t="str">
-        <v>SNW-3398-01</v>
+        <v>SNW-2905-01</v>
       </c>
       <c r="D31" t="str">
-        <v>SNW-5-01</v>
+        <v>SNW-7-01</v>
       </c>
       <c r="E31" t="str">
-        <v>SNW-Image5-05</v>
+        <v>SNW-Image7-01</v>
       </c>
       <c r="F31" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-5-01/4.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-7-01/0.jpg</v>
       </c>
       <c r="G31" t="str">
         <v>700</v>
@@ -1213,19 +1217,19 @@
         <v>image</v>
       </c>
       <c r="B32" t="str">
-        <v>snowboard106</v>
+        <v>snowboard107</v>
       </c>
       <c r="C32" t="str">
-        <v>SNW-2245-01</v>
+        <v>SNW-2905-01</v>
       </c>
       <c r="D32" t="str">
-        <v>SNW-6-01</v>
+        <v>SNW-7-01</v>
       </c>
       <c r="E32" t="str">
-        <v>SNW-Image6-01</v>
+        <v>SNW-Image7-02</v>
       </c>
       <c r="F32" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-6-01/0.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-7-01/1.jpg</v>
       </c>
       <c r="G32" t="str">
         <v>700</v>
@@ -1239,19 +1243,19 @@
         <v>image</v>
       </c>
       <c r="B33" t="str">
-        <v>snowboard106</v>
+        <v>snowboard107</v>
       </c>
       <c r="C33" t="str">
-        <v>SNW-2245-01</v>
+        <v>SNW-2905-01</v>
       </c>
       <c r="D33" t="str">
-        <v>SNW-6-01</v>
+        <v>SNW-7-01</v>
       </c>
       <c r="E33" t="str">
-        <v>SNW-Image6-02</v>
+        <v>SNW-Image7-03</v>
       </c>
       <c r="F33" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-6-01/1.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-7-01/2.jpg</v>
       </c>
       <c r="G33" t="str">
         <v>700</v>
@@ -1265,19 +1269,19 @@
         <v>image</v>
       </c>
       <c r="B34" t="str">
-        <v>snowboard106</v>
+        <v>snowboard107</v>
       </c>
       <c r="C34" t="str">
-        <v>SNW-2245-01</v>
+        <v>SNW-2905-01</v>
       </c>
       <c r="D34" t="str">
-        <v>SNW-6-01</v>
+        <v>SNW-7-01</v>
       </c>
       <c r="E34" t="str">
-        <v>SNW-Image6-03</v>
+        <v>SNW-Image7-04</v>
       </c>
       <c r="F34" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-6-01/2.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-7-01/3.jpg</v>
       </c>
       <c r="G34" t="str">
         <v>700</v>
@@ -1291,19 +1295,19 @@
         <v>image</v>
       </c>
       <c r="B35" t="str">
-        <v>snowboard106</v>
+        <v>snowboard107</v>
       </c>
       <c r="C35" t="str">
-        <v>SNW-2245-01</v>
+        <v>SNW-2905-01</v>
       </c>
       <c r="D35" t="str">
-        <v>SNW-6-01</v>
+        <v>SNW-7-01</v>
       </c>
       <c r="E35" t="str">
-        <v>SNW-Image6-04</v>
+        <v>SNW-Image7-05</v>
       </c>
       <c r="F35" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-6-01/3.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-7-01/4.jpg</v>
       </c>
       <c r="G35" t="str">
         <v>700</v>
@@ -1317,19 +1321,19 @@
         <v>image</v>
       </c>
       <c r="B36" t="str">
-        <v>snowboard106</v>
+        <v>snowboard108</v>
       </c>
       <c r="C36" t="str">
-        <v>SNW-2245-01</v>
+        <v>SNW-3162-01</v>
       </c>
       <c r="D36" t="str">
-        <v>SNW-6-01</v>
+        <v>SNW-8-01</v>
       </c>
       <c r="E36" t="str">
-        <v>SNW-Image6-05</v>
+        <v>SNW-Image8-01</v>
       </c>
       <c r="F36" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-6-01/4.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-8-01/0.jpg</v>
       </c>
       <c r="G36" t="str">
         <v>700</v>
@@ -1343,19 +1347,19 @@
         <v>image</v>
       </c>
       <c r="B37" t="str">
-        <v>snowboard107</v>
+        <v>snowboard108</v>
       </c>
       <c r="C37" t="str">
-        <v>SNW-2905-01</v>
+        <v>SNW-3162-01</v>
       </c>
       <c r="D37" t="str">
-        <v>SNW-7-01</v>
+        <v>SNW-8-01</v>
       </c>
       <c r="E37" t="str">
-        <v>SNW-Image7-01</v>
+        <v>SNW-Image8-02</v>
       </c>
       <c r="F37" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-7-01/0.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-8-01/1.jpg</v>
       </c>
       <c r="G37" t="str">
         <v>700</v>
@@ -1369,19 +1373,19 @@
         <v>image</v>
       </c>
       <c r="B38" t="str">
-        <v>snowboard107</v>
+        <v>snowboard108</v>
       </c>
       <c r="C38" t="str">
-        <v>SNW-2905-01</v>
+        <v>SNW-3162-01</v>
       </c>
       <c r="D38" t="str">
-        <v>SNW-7-01</v>
+        <v>SNW-8-01</v>
       </c>
       <c r="E38" t="str">
-        <v>SNW-Image7-02</v>
+        <v>SNW-Image8-03</v>
       </c>
       <c r="F38" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-7-01/1.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-8-01/2.jpg</v>
       </c>
       <c r="G38" t="str">
         <v>700</v>
@@ -1395,19 +1399,19 @@
         <v>image</v>
       </c>
       <c r="B39" t="str">
-        <v>snowboard107</v>
+        <v>snowboard109</v>
       </c>
       <c r="C39" t="str">
-        <v>SNW-2905-01</v>
+        <v>SNW-2858-01</v>
       </c>
       <c r="D39" t="str">
-        <v>SNW-7-01</v>
+        <v>SNW-9-01</v>
       </c>
       <c r="E39" t="str">
-        <v>SNW-Image7-03</v>
+        <v>SNW-Image9-01</v>
       </c>
       <c r="F39" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-7-01/2.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-9-01/0.jpg</v>
       </c>
       <c r="G39" t="str">
         <v>700</v>
@@ -1421,19 +1425,19 @@
         <v>image</v>
       </c>
       <c r="B40" t="str">
-        <v>snowboard107</v>
+        <v>snowboard109</v>
       </c>
       <c r="C40" t="str">
-        <v>SNW-2905-01</v>
+        <v>SNW-2858-01</v>
       </c>
       <c r="D40" t="str">
-        <v>SNW-7-01</v>
+        <v>SNW-9-01</v>
       </c>
       <c r="E40" t="str">
-        <v>SNW-Image7-04</v>
+        <v>SNW-Image9-02</v>
       </c>
       <c r="F40" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-7-01/3.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-9-01/1.jpg</v>
       </c>
       <c r="G40" t="str">
         <v>700</v>
@@ -1447,19 +1451,19 @@
         <v>image</v>
       </c>
       <c r="B41" t="str">
-        <v>snowboard107</v>
+        <v>snowboard109</v>
       </c>
       <c r="C41" t="str">
-        <v>SNW-2905-01</v>
+        <v>SNW-2858-01</v>
       </c>
       <c r="D41" t="str">
-        <v>SNW-7-01</v>
+        <v>SNW-9-01</v>
       </c>
       <c r="E41" t="str">
-        <v>SNW-Image7-05</v>
+        <v>SNW-Image9-03</v>
       </c>
       <c r="F41" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-7-01/4.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-9-01/2.jpg</v>
       </c>
       <c r="G41" t="str">
         <v>700</v>
@@ -1473,19 +1477,19 @@
         <v>image</v>
       </c>
       <c r="B42" t="str">
-        <v>snowboard108</v>
+        <v>snowboard109</v>
       </c>
       <c r="C42" t="str">
-        <v>SNW-3162-01</v>
+        <v>SNW-2858-01</v>
       </c>
       <c r="D42" t="str">
-        <v>SNW-8-01</v>
+        <v>SNW-9-01</v>
       </c>
       <c r="E42" t="str">
-        <v>SNW-Image8-01</v>
+        <v>SNW-Image9-04</v>
       </c>
       <c r="F42" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-8-01/0.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-9-01/3.jpg</v>
       </c>
       <c r="G42" t="str">
         <v>700</v>
@@ -1499,238 +1503,30 @@
         <v>image</v>
       </c>
       <c r="B43" t="str">
-        <v>snowboard108</v>
+        <v>snowboard109</v>
       </c>
       <c r="C43" t="str">
-        <v>SNW-3162-01</v>
+        <v>SNW-2858-01</v>
       </c>
       <c r="D43" t="str">
-        <v>SNW-8-01</v>
+        <v>SNW-9-01</v>
       </c>
       <c r="E43" t="str">
-        <v>SNW-Image8-02</v>
+        <v>SNW-Image9-05</v>
       </c>
       <c r="F43" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-8-01/1.jpg</v>
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-9-01/4.jpg</v>
       </c>
       <c r="G43" t="str">
         <v>700</v>
       </c>
       <c r="H43" t="str">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="str">
-        <v>image</v>
-      </c>
-      <c r="B44" t="str">
-        <v>snowboard108</v>
-      </c>
-      <c r="C44" t="str">
-        <v>SNW-3162-01</v>
-      </c>
-      <c r="D44" t="str">
-        <v>SNW-8-01</v>
-      </c>
-      <c r="E44" t="str">
-        <v>SNW-Image8-03</v>
-      </c>
-      <c r="F44" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-8-01/2.jpg</v>
-      </c>
-      <c r="G44" t="str">
-        <v>700</v>
-      </c>
-      <c r="H44" t="str">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="str">
-        <v>image</v>
-      </c>
-      <c r="B45" t="str">
-        <v>snowboard108</v>
-      </c>
-      <c r="C45" t="str">
-        <v>SNW-3162-01</v>
-      </c>
-      <c r="D45" t="str">
-        <v>SNW-8-01</v>
-      </c>
-      <c r="E45" t="str">
-        <v>SNW-Image8-04</v>
-      </c>
-      <c r="F45" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-8-01/3.jpg</v>
-      </c>
-      <c r="G45" t="str">
-        <v>700</v>
-      </c>
-      <c r="H45" t="str">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="str">
-        <v>image</v>
-      </c>
-      <c r="B46" t="str">
-        <v>snowboard108</v>
-      </c>
-      <c r="C46" t="str">
-        <v>SNW-3162-01</v>
-      </c>
-      <c r="D46" t="str">
-        <v>SNW-8-01</v>
-      </c>
-      <c r="E46" t="str">
-        <v>SNW-Image8-05</v>
-      </c>
-      <c r="F46" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-8-01/4.jpg</v>
-      </c>
-      <c r="G46" t="str">
-        <v>700</v>
-      </c>
-      <c r="H46" t="str">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="str">
-        <v>image</v>
-      </c>
-      <c r="B47" t="str">
-        <v>snowboard109</v>
-      </c>
-      <c r="C47" t="str">
-        <v>SNW-2858-01</v>
-      </c>
-      <c r="D47" t="str">
-        <v>SNW-9-01</v>
-      </c>
-      <c r="E47" t="str">
-        <v>SNW-Image9-01</v>
-      </c>
-      <c r="F47" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-9-01/0.jpg</v>
-      </c>
-      <c r="G47" t="str">
-        <v>700</v>
-      </c>
-      <c r="H47" t="str">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="str">
-        <v>image</v>
-      </c>
-      <c r="B48" t="str">
-        <v>snowboard109</v>
-      </c>
-      <c r="C48" t="str">
-        <v>SNW-2858-01</v>
-      </c>
-      <c r="D48" t="str">
-        <v>SNW-9-01</v>
-      </c>
-      <c r="E48" t="str">
-        <v>SNW-Image9-02</v>
-      </c>
-      <c r="F48" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-9-01/1.jpg</v>
-      </c>
-      <c r="G48" t="str">
-        <v>700</v>
-      </c>
-      <c r="H48" t="str">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="str">
-        <v>image</v>
-      </c>
-      <c r="B49" t="str">
-        <v>snowboard109</v>
-      </c>
-      <c r="C49" t="str">
-        <v>SNW-2858-01</v>
-      </c>
-      <c r="D49" t="str">
-        <v>SNW-9-01</v>
-      </c>
-      <c r="E49" t="str">
-        <v>SNW-Image9-03</v>
-      </c>
-      <c r="F49" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-9-01/2.jpg</v>
-      </c>
-      <c r="G49" t="str">
-        <v>700</v>
-      </c>
-      <c r="H49" t="str">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="str">
-        <v>image</v>
-      </c>
-      <c r="B50" t="str">
-        <v>snowboard109</v>
-      </c>
-      <c r="C50" t="str">
-        <v>SNW-2858-01</v>
-      </c>
-      <c r="D50" t="str">
-        <v>SNW-9-01</v>
-      </c>
-      <c r="E50" t="str">
-        <v>SNW-Image9-04</v>
-      </c>
-      <c r="F50" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-9-01/3.jpg</v>
-      </c>
-      <c r="G50" t="str">
-        <v>700</v>
-      </c>
-      <c r="H50" t="str">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="str">
-        <v>image</v>
-      </c>
-      <c r="B51" t="str">
-        <v>snowboard109</v>
-      </c>
-      <c r="C51" t="str">
-        <v>SNW-2858-01</v>
-      </c>
-      <c r="D51" t="str">
-        <v>SNW-9-01</v>
-      </c>
-      <c r="E51" t="str">
-        <v>SNW-Image9-05</v>
-      </c>
-      <c r="F51" t="str">
-        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-9-01/4.jpg</v>
-      </c>
-      <c r="G51" t="str">
-        <v>700</v>
-      </c>
-      <c r="H51" t="str">
         <v>700</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H51"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H43"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: scale the parse to 20 objects
</commit_message>
<xml_diff>
--- a/Assets.xlsx
+++ b/Assets.xlsx
@@ -397,14 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H79"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <cols>
-    <col min="1" max="1" width="13.83203125" customWidth="1"/>
-    <col min="8" max="8" width="5.83203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -1524,9 +1520,945 @@
         <v>700</v>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>image</v>
+      </c>
+      <c r="B44" t="str">
+        <v>snowboard1010</v>
+      </c>
+      <c r="C44" t="str">
+        <v>SNW-2015-01</v>
+      </c>
+      <c r="D44" t="str">
+        <v>SNW-10-01</v>
+      </c>
+      <c r="E44" t="str">
+        <v>SNW-Image10-01</v>
+      </c>
+      <c r="F44" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-10-01/0.jpg</v>
+      </c>
+      <c r="G44" t="str">
+        <v>700</v>
+      </c>
+      <c r="H44" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>image</v>
+      </c>
+      <c r="B45" t="str">
+        <v>snowboard1010</v>
+      </c>
+      <c r="C45" t="str">
+        <v>SNW-2015-01</v>
+      </c>
+      <c r="D45" t="str">
+        <v>SNW-10-01</v>
+      </c>
+      <c r="E45" t="str">
+        <v>SNW-Image10-02</v>
+      </c>
+      <c r="F45" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-10-01/1.jpg</v>
+      </c>
+      <c r="G45" t="str">
+        <v>700</v>
+      </c>
+      <c r="H45" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>image</v>
+      </c>
+      <c r="B46" t="str">
+        <v>snowboard1010</v>
+      </c>
+      <c r="C46" t="str">
+        <v>SNW-2015-01</v>
+      </c>
+      <c r="D46" t="str">
+        <v>SNW-10-01</v>
+      </c>
+      <c r="E46" t="str">
+        <v>SNW-Image10-03</v>
+      </c>
+      <c r="F46" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-10-01/2.jpg</v>
+      </c>
+      <c r="G46" t="str">
+        <v>700</v>
+      </c>
+      <c r="H46" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>image</v>
+      </c>
+      <c r="B47" t="str">
+        <v>snowboard1010</v>
+      </c>
+      <c r="C47" t="str">
+        <v>SNW-2015-01</v>
+      </c>
+      <c r="D47" t="str">
+        <v>SNW-10-01</v>
+      </c>
+      <c r="E47" t="str">
+        <v>SNW-Image10-04</v>
+      </c>
+      <c r="F47" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-10-01/3.jpg</v>
+      </c>
+      <c r="G47" t="str">
+        <v>700</v>
+      </c>
+      <c r="H47" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>image</v>
+      </c>
+      <c r="B48" t="str">
+        <v>snowboard1010</v>
+      </c>
+      <c r="C48" t="str">
+        <v>SNW-2015-01</v>
+      </c>
+      <c r="D48" t="str">
+        <v>SNW-10-01</v>
+      </c>
+      <c r="E48" t="str">
+        <v>SNW-Image10-05</v>
+      </c>
+      <c r="F48" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-10-01/4.jpg</v>
+      </c>
+      <c r="G48" t="str">
+        <v>700</v>
+      </c>
+      <c r="H48" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>image</v>
+      </c>
+      <c r="B49" t="str">
+        <v>snowboard1011</v>
+      </c>
+      <c r="C49" t="str">
+        <v>SNW-3475-01</v>
+      </c>
+      <c r="D49" t="str">
+        <v>SNW-11-01</v>
+      </c>
+      <c r="E49" t="str">
+        <v>SNW-Image11-01</v>
+      </c>
+      <c r="F49" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-11-01/0.jpg</v>
+      </c>
+      <c r="G49" t="str">
+        <v>700</v>
+      </c>
+      <c r="H49" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>image</v>
+      </c>
+      <c r="B50" t="str">
+        <v>snowboard1012</v>
+      </c>
+      <c r="C50" t="str">
+        <v>SNW-2784-01</v>
+      </c>
+      <c r="D50" t="str">
+        <v>SNW-12-01</v>
+      </c>
+      <c r="E50" t="str">
+        <v>SNW-Image12-01</v>
+      </c>
+      <c r="F50" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-12-01/0.jpg</v>
+      </c>
+      <c r="G50" t="str">
+        <v>700</v>
+      </c>
+      <c r="H50" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>image</v>
+      </c>
+      <c r="B51" t="str">
+        <v>snowboard1012</v>
+      </c>
+      <c r="C51" t="str">
+        <v>SNW-2784-01</v>
+      </c>
+      <c r="D51" t="str">
+        <v>SNW-12-01</v>
+      </c>
+      <c r="E51" t="str">
+        <v>SNW-Image12-02</v>
+      </c>
+      <c r="F51" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-12-01/1.jpg</v>
+      </c>
+      <c r="G51" t="str">
+        <v>700</v>
+      </c>
+      <c r="H51" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>image</v>
+      </c>
+      <c r="B52" t="str">
+        <v>snowboard1012</v>
+      </c>
+      <c r="C52" t="str">
+        <v>SNW-2784-01</v>
+      </c>
+      <c r="D52" t="str">
+        <v>SNW-12-01</v>
+      </c>
+      <c r="E52" t="str">
+        <v>SNW-Image12-03</v>
+      </c>
+      <c r="F52" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-12-01/2.jpg</v>
+      </c>
+      <c r="G52" t="str">
+        <v>700</v>
+      </c>
+      <c r="H52" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>image</v>
+      </c>
+      <c r="B53" t="str">
+        <v>snowboard1012</v>
+      </c>
+      <c r="C53" t="str">
+        <v>SNW-2784-01</v>
+      </c>
+      <c r="D53" t="str">
+        <v>SNW-12-01</v>
+      </c>
+      <c r="E53" t="str">
+        <v>SNW-Image12-04</v>
+      </c>
+      <c r="F53" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-12-01/3.jpg</v>
+      </c>
+      <c r="G53" t="str">
+        <v>700</v>
+      </c>
+      <c r="H53" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>image</v>
+      </c>
+      <c r="B54" t="str">
+        <v>snowboard1012</v>
+      </c>
+      <c r="C54" t="str">
+        <v>SNW-2784-01</v>
+      </c>
+      <c r="D54" t="str">
+        <v>SNW-12-01</v>
+      </c>
+      <c r="E54" t="str">
+        <v>SNW-Image12-05</v>
+      </c>
+      <c r="F54" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-12-01/4.jpg</v>
+      </c>
+      <c r="G54" t="str">
+        <v>700</v>
+      </c>
+      <c r="H54" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>image</v>
+      </c>
+      <c r="B55" t="str">
+        <v>snowboard1013</v>
+      </c>
+      <c r="C55" t="str">
+        <v>SNW-3275-01</v>
+      </c>
+      <c r="D55" t="str">
+        <v>SNW-13-01</v>
+      </c>
+      <c r="E55" t="str">
+        <v>SNW-Image13-01</v>
+      </c>
+      <c r="F55" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-13-01/0.jpg</v>
+      </c>
+      <c r="G55" t="str">
+        <v>700</v>
+      </c>
+      <c r="H55" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>image</v>
+      </c>
+      <c r="B56" t="str">
+        <v>snowboard1013</v>
+      </c>
+      <c r="C56" t="str">
+        <v>SNW-3275-01</v>
+      </c>
+      <c r="D56" t="str">
+        <v>SNW-13-01</v>
+      </c>
+      <c r="E56" t="str">
+        <v>SNW-Image13-02</v>
+      </c>
+      <c r="F56" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-13-01/1.jpg</v>
+      </c>
+      <c r="G56" t="str">
+        <v>700</v>
+      </c>
+      <c r="H56" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>image</v>
+      </c>
+      <c r="B57" t="str">
+        <v>snowboard1013</v>
+      </c>
+      <c r="C57" t="str">
+        <v>SNW-3275-01</v>
+      </c>
+      <c r="D57" t="str">
+        <v>SNW-13-01</v>
+      </c>
+      <c r="E57" t="str">
+        <v>SNW-Image13-03</v>
+      </c>
+      <c r="F57" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-13-01/2.jpg</v>
+      </c>
+      <c r="G57" t="str">
+        <v>700</v>
+      </c>
+      <c r="H57" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>image</v>
+      </c>
+      <c r="B58" t="str">
+        <v>snowboard1013</v>
+      </c>
+      <c r="C58" t="str">
+        <v>SNW-3275-01</v>
+      </c>
+      <c r="D58" t="str">
+        <v>SNW-13-01</v>
+      </c>
+      <c r="E58" t="str">
+        <v>SNW-Image13-04</v>
+      </c>
+      <c r="F58" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-13-01/3.jpg</v>
+      </c>
+      <c r="G58" t="str">
+        <v>700</v>
+      </c>
+      <c r="H58" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>image</v>
+      </c>
+      <c r="B59" t="str">
+        <v>snowboard1013</v>
+      </c>
+      <c r="C59" t="str">
+        <v>SNW-3275-01</v>
+      </c>
+      <c r="D59" t="str">
+        <v>SNW-13-01</v>
+      </c>
+      <c r="E59" t="str">
+        <v>SNW-Image13-05</v>
+      </c>
+      <c r="F59" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-13-01/4.jpg</v>
+      </c>
+      <c r="G59" t="str">
+        <v>700</v>
+      </c>
+      <c r="H59" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>image</v>
+      </c>
+      <c r="B60" t="str">
+        <v>snowboard1014</v>
+      </c>
+      <c r="C60" t="str">
+        <v>SNW-3655-01</v>
+      </c>
+      <c r="D60" t="str">
+        <v>SNW-14-01</v>
+      </c>
+      <c r="E60" t="str">
+        <v>SNW-Image14-01</v>
+      </c>
+      <c r="F60" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-14-01/0.jpg</v>
+      </c>
+      <c r="G60" t="str">
+        <v>700</v>
+      </c>
+      <c r="H60" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>image</v>
+      </c>
+      <c r="B61" t="str">
+        <v>snowboard1015</v>
+      </c>
+      <c r="C61" t="str">
+        <v>SNW-3820-01</v>
+      </c>
+      <c r="D61" t="str">
+        <v>SNW-15-01</v>
+      </c>
+      <c r="E61" t="str">
+        <v>SNW-Image15-01</v>
+      </c>
+      <c r="F61" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-15-01/0.jpg</v>
+      </c>
+      <c r="G61" t="str">
+        <v>700</v>
+      </c>
+      <c r="H61" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>image</v>
+      </c>
+      <c r="B62" t="str">
+        <v>snowboard1016</v>
+      </c>
+      <c r="C62" t="str">
+        <v>SNW-2578-01</v>
+      </c>
+      <c r="D62" t="str">
+        <v>SNW-16-01</v>
+      </c>
+      <c r="E62" t="str">
+        <v>SNW-Image16-01</v>
+      </c>
+      <c r="F62" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-16-01/0.jpg</v>
+      </c>
+      <c r="G62" t="str">
+        <v>700</v>
+      </c>
+      <c r="H62" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>image</v>
+      </c>
+      <c r="B63" t="str">
+        <v>snowboard1016</v>
+      </c>
+      <c r="C63" t="str">
+        <v>SNW-2578-01</v>
+      </c>
+      <c r="D63" t="str">
+        <v>SNW-16-01</v>
+      </c>
+      <c r="E63" t="str">
+        <v>SNW-Image16-02</v>
+      </c>
+      <c r="F63" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-16-01/1.jpg</v>
+      </c>
+      <c r="G63" t="str">
+        <v>700</v>
+      </c>
+      <c r="H63" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>image</v>
+      </c>
+      <c r="B64" t="str">
+        <v>snowboard1016</v>
+      </c>
+      <c r="C64" t="str">
+        <v>SNW-2578-01</v>
+      </c>
+      <c r="D64" t="str">
+        <v>SNW-16-01</v>
+      </c>
+      <c r="E64" t="str">
+        <v>SNW-Image16-03</v>
+      </c>
+      <c r="F64" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-16-01/2.jpg</v>
+      </c>
+      <c r="G64" t="str">
+        <v>700</v>
+      </c>
+      <c r="H64" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>image</v>
+      </c>
+      <c r="B65" t="str">
+        <v>snowboard1016</v>
+      </c>
+      <c r="C65" t="str">
+        <v>SNW-2578-01</v>
+      </c>
+      <c r="D65" t="str">
+        <v>SNW-16-01</v>
+      </c>
+      <c r="E65" t="str">
+        <v>SNW-Image16-04</v>
+      </c>
+      <c r="F65" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-16-01/3.jpg</v>
+      </c>
+      <c r="G65" t="str">
+        <v>700</v>
+      </c>
+      <c r="H65" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>image</v>
+      </c>
+      <c r="B66" t="str">
+        <v>snowboard1016</v>
+      </c>
+      <c r="C66" t="str">
+        <v>SNW-2578-01</v>
+      </c>
+      <c r="D66" t="str">
+        <v>SNW-16-01</v>
+      </c>
+      <c r="E66" t="str">
+        <v>SNW-Image16-05</v>
+      </c>
+      <c r="F66" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-16-01/4.jpg</v>
+      </c>
+      <c r="G66" t="str">
+        <v>700</v>
+      </c>
+      <c r="H66" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>image</v>
+      </c>
+      <c r="B67" t="str">
+        <v>snowboard1017</v>
+      </c>
+      <c r="C67" t="str">
+        <v>SNW-3321-01</v>
+      </c>
+      <c r="D67" t="str">
+        <v>SNW-17-01</v>
+      </c>
+      <c r="E67" t="str">
+        <v>SNW-Image17-01</v>
+      </c>
+      <c r="F67" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-17-01/0.jpg</v>
+      </c>
+      <c r="G67" t="str">
+        <v>700</v>
+      </c>
+      <c r="H67" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>image</v>
+      </c>
+      <c r="B68" t="str">
+        <v>snowboard1017</v>
+      </c>
+      <c r="C68" t="str">
+        <v>SNW-3321-01</v>
+      </c>
+      <c r="D68" t="str">
+        <v>SNW-17-01</v>
+      </c>
+      <c r="E68" t="str">
+        <v>SNW-Image17-02</v>
+      </c>
+      <c r="F68" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-17-01/1.jpg</v>
+      </c>
+      <c r="G68" t="str">
+        <v>700</v>
+      </c>
+      <c r="H68" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>image</v>
+      </c>
+      <c r="B69" t="str">
+        <v>snowboard1017</v>
+      </c>
+      <c r="C69" t="str">
+        <v>SNW-3321-01</v>
+      </c>
+      <c r="D69" t="str">
+        <v>SNW-17-01</v>
+      </c>
+      <c r="E69" t="str">
+        <v>SNW-Image17-03</v>
+      </c>
+      <c r="F69" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-17-01/2.jpg</v>
+      </c>
+      <c r="G69" t="str">
+        <v>700</v>
+      </c>
+      <c r="H69" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>image</v>
+      </c>
+      <c r="B70" t="str">
+        <v>snowboard1017</v>
+      </c>
+      <c r="C70" t="str">
+        <v>SNW-3321-01</v>
+      </c>
+      <c r="D70" t="str">
+        <v>SNW-17-01</v>
+      </c>
+      <c r="E70" t="str">
+        <v>SNW-Image17-04</v>
+      </c>
+      <c r="F70" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-17-01/3.jpg</v>
+      </c>
+      <c r="G70" t="str">
+        <v>700</v>
+      </c>
+      <c r="H70" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>image</v>
+      </c>
+      <c r="B71" t="str">
+        <v>snowboard1017</v>
+      </c>
+      <c r="C71" t="str">
+        <v>SNW-3321-01</v>
+      </c>
+      <c r="D71" t="str">
+        <v>SNW-17-01</v>
+      </c>
+      <c r="E71" t="str">
+        <v>SNW-Image17-05</v>
+      </c>
+      <c r="F71" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-17-01/4.jpg</v>
+      </c>
+      <c r="G71" t="str">
+        <v>700</v>
+      </c>
+      <c r="H71" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>image</v>
+      </c>
+      <c r="B72" t="str">
+        <v>snowboard1018</v>
+      </c>
+      <c r="C72" t="str">
+        <v>SNW-3658-01</v>
+      </c>
+      <c r="D72" t="str">
+        <v>SNW-18-01</v>
+      </c>
+      <c r="E72" t="str">
+        <v>SNW-Image18-01</v>
+      </c>
+      <c r="F72" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-18-01/0.jpg</v>
+      </c>
+      <c r="G72" t="str">
+        <v>700</v>
+      </c>
+      <c r="H72" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>image</v>
+      </c>
+      <c r="B73" t="str">
+        <v>snowboard1018</v>
+      </c>
+      <c r="C73" t="str">
+        <v>SNW-3658-01</v>
+      </c>
+      <c r="D73" t="str">
+        <v>SNW-18-01</v>
+      </c>
+      <c r="E73" t="str">
+        <v>SNW-Image18-02</v>
+      </c>
+      <c r="F73" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-18-01/1.jpg</v>
+      </c>
+      <c r="G73" t="str">
+        <v>700</v>
+      </c>
+      <c r="H73" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>image</v>
+      </c>
+      <c r="B74" t="str">
+        <v>snowboard1018</v>
+      </c>
+      <c r="C74" t="str">
+        <v>SNW-3658-01</v>
+      </c>
+      <c r="D74" t="str">
+        <v>SNW-18-01</v>
+      </c>
+      <c r="E74" t="str">
+        <v>SNW-Image18-03</v>
+      </c>
+      <c r="F74" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-18-01/2.jpg</v>
+      </c>
+      <c r="G74" t="str">
+        <v>700</v>
+      </c>
+      <c r="H74" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>image</v>
+      </c>
+      <c r="B75" t="str">
+        <v>snowboard1018</v>
+      </c>
+      <c r="C75" t="str">
+        <v>SNW-3658-01</v>
+      </c>
+      <c r="D75" t="str">
+        <v>SNW-18-01</v>
+      </c>
+      <c r="E75" t="str">
+        <v>SNW-Image18-04</v>
+      </c>
+      <c r="F75" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-18-01/3.jpg</v>
+      </c>
+      <c r="G75" t="str">
+        <v>700</v>
+      </c>
+      <c r="H75" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>image</v>
+      </c>
+      <c r="B76" t="str">
+        <v>snowboard1018</v>
+      </c>
+      <c r="C76" t="str">
+        <v>SNW-3658-01</v>
+      </c>
+      <c r="D76" t="str">
+        <v>SNW-18-01</v>
+      </c>
+      <c r="E76" t="str">
+        <v>SNW-Image18-05</v>
+      </c>
+      <c r="F76" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-18-01/4.jpg</v>
+      </c>
+      <c r="G76" t="str">
+        <v>700</v>
+      </c>
+      <c r="H76" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>image</v>
+      </c>
+      <c r="B77" t="str">
+        <v>snowboard1019</v>
+      </c>
+      <c r="C77" t="str">
+        <v>SNW-2798-01</v>
+      </c>
+      <c r="D77" t="str">
+        <v>SNW-19-01</v>
+      </c>
+      <c r="E77" t="str">
+        <v>SNW-Image19-01</v>
+      </c>
+      <c r="F77" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-19-01/0.jpg</v>
+      </c>
+      <c r="G77" t="str">
+        <v>700</v>
+      </c>
+      <c r="H77" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>image</v>
+      </c>
+      <c r="B78" t="str">
+        <v>snowboard1019</v>
+      </c>
+      <c r="C78" t="str">
+        <v>SNW-2798-01</v>
+      </c>
+      <c r="D78" t="str">
+        <v>SNW-19-01</v>
+      </c>
+      <c r="E78" t="str">
+        <v>SNW-Image19-02</v>
+      </c>
+      <c r="F78" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-19-01/1.jpg</v>
+      </c>
+      <c r="G78" t="str">
+        <v>700</v>
+      </c>
+      <c r="H78" t="str">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>image</v>
+      </c>
+      <c r="B79" t="str">
+        <v>snowboard1019</v>
+      </c>
+      <c r="C79" t="str">
+        <v>SNW-2798-01</v>
+      </c>
+      <c r="D79" t="str">
+        <v>SNW-19-01</v>
+      </c>
+      <c r="E79" t="str">
+        <v>SNW-Image19-03</v>
+      </c>
+      <c r="F79" t="str">
+        <v>https://raw.githubusercontent.com/ksarise/parser/main/assets/SNW-19-01/2.jpg</v>
+      </c>
+      <c r="G79" t="str">
+        <v>700</v>
+      </c>
+      <c r="H79" t="str">
+        <v>700</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H43"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H79"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>